<commit_message>
Updated ISL model - 2025-08-01 01:06
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/SuppXLS/scen_tsparameters_ts_192.xlsx
+++ b/VerveStacks_ISL/SuppXLS/scen_tsparameters_ts_192.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ISL\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE97613-E5CA-47AD-941B-304F001DD566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13954D32-8A68-41A5-A443-451E058CBDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -1683,10 +1683,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Rah18,Rc0416h11,Wb0121h13,Rc0416h14,Rc0416h17,Sah10,Se0716h18,Tah09,Tg1016h11,Rc0416h07,Sah13,Sah16,Tg1016h13,Wah07,Wah16,Wb0121h09,Rah16,Sah08,Tah17,Wb0121h15,Wb0121h17,Rah07,Rc0416h08,Se0716h15,Se0716h17,Tg1016h14,Tg1016h15,Tg1016h16,Tg1016h17,Wah09,Wb0121h10,Rc0416h09,Sah07,Tah16,Tah18,Wah15,Wb0121h14,Wb0121h16,Rah17,Rc0416h10,Se0716h07,Tah11,Wb0121h12,Sah12,Se0716h09,Se0716h11,Tah10,Wb0121h11,Rah08,Rah10,Rc0416h16,Sah14,Sah17,Sah18,Se0716h12,Tah15,Tg1016h08,Wah08,Wah18,Sah15,Se0716h08,Se0716h13,Tg1016h09,Wah13,Rah15,Sah09,Rah13,Tah08,Wb0121h07,Rc0416h12,Se0716h10,Tg1016h07,Wah11,Rc0416h18,Se0716h14,Tah07,Tah12,Tg1016h12,Wah17,Rah12,Rah14,Rc0416h13,Tah13,Tg1016h18,Wah12,Rah09,Rah11,Rc0416h15,Sah11,Se0716h16,Tah14,Tg1016h10,Wah10,Wah14,Wb0121h08,Wb0121h18</t>
-  </si>
-  <si>
-    <t>Sah04,Se0716h24,Tah02,Tah05,Tg1016h03,Tg1016h04,Wah05,Rah05,Rc0416h06,Rc0416h22,Rc0416h23,Sah20,Sah21,Sah22,Se0716h21,Tg1016h24,Wah20,Wb0121h21,Wb0121h23,Rah01,Rah04,Rc0416h01,Rc0416h04,Se0716h02,Se0716h20,Tah06,Wah23,Wb0121h20,Rc0416h05,Se0716h06,Tg1016h06,Wb0121h03,Wb0121h04,Rah23,Rah24,Sah03,Sah05,Sah19,Wah22,Rah03,Rc0416h02,Wah21,Sah23,Sah24,Se0716h04,Tg1016h01,Wah02,Wah19,Wb0121h01,Tah20,Tg1016h23,Wah24,Wb0121h02,Wb0121h06,Rah02,Rah20,Wah01,Se0716h23,Tg1016h19,Tg1016h21,Wah03,Rah06,Rah21,Rc0416h24,Tah24,Tg1016h20,Rc0416h20,Se0716h22,Tg1016h02,Tg1016h22,Wah06,Rc0416h03,Rc0416h21,Se0716h19,Tah03,Tah04,Wah04,Rah19,Se0716h01,Se0716h03,Se0716h05,Tah01,Tah19,Tah22,Rah22,Sah02,Sah06,Tah23,Wb0121h19,Wb0121h22,Rc0416h19,Sah01,Tah21,Tg1016h05,Wb0121h05,Wb0121h24</t>
+    <t>Rah13,Tah08,Wb0121h07,Rah12,Rah14,Rc0416h13,Tah13,Tg1016h18,Wah12,Rc0416h14,Rc0416h17,Sah10,Se0716h18,Tah09,Tg1016h11,Rah17,Rc0416h10,Se0716h07,Tah11,Wb0121h12,Rah07,Rc0416h08,Se0716h15,Se0716h17,Tg1016h14,Tg1016h15,Tg1016h16,Tg1016h17,Wah09,Wb0121h10,Rah09,Rah11,Rc0416h15,Sah11,Se0716h16,Tah14,Tg1016h10,Wah10,Wah14,Wb0121h08,Wb0121h18,Rc0416h18,Se0716h14,Tah07,Tah12,Tg1016h12,Wah17,Sah15,Se0716h08,Se0716h13,Tg1016h09,Wah13,Rc0416h09,Sah07,Tah16,Tah18,Wah15,Wb0121h14,Wb0121h16,Rah15,Sah09,Rah08,Rah10,Rc0416h16,Sah14,Sah17,Sah18,Se0716h12,Tah15,Tg1016h08,Wah08,Wah18,Rc0416h12,Se0716h10,Tg1016h07,Wah11,Rc0416h07,Sah13,Sah16,Tg1016h13,Wah07,Wah16,Wb0121h09,Rah18,Rc0416h11,Wb0121h13,Sah12,Se0716h09,Se0716h11,Tah10,Wb0121h11,Rah16,Sah08,Tah17,Wb0121h15,Wb0121h17</t>
+  </si>
+  <si>
+    <t>Rc0416h20,Se0716h22,Tg1016h02,Tg1016h22,Wah06,Rah22,Sah02,Sah06,Tah23,Wb0121h19,Wb0121h22,Rah05,Rc0416h06,Rc0416h22,Rc0416h23,Sah20,Sah21,Sah22,Se0716h21,Tg1016h24,Wah20,Wb0121h21,Wb0121h23,Sah23,Sah24,Se0716h04,Tg1016h01,Wah02,Wah19,Wb0121h01,Rah23,Rah24,Sah03,Sah05,Sah19,Wah22,Rc0416h19,Sah01,Tah21,Tg1016h05,Wb0121h05,Wb0121h24,Rah19,Se0716h01,Se0716h03,Se0716h05,Tah01,Tah19,Tah22,Se0716h23,Tg1016h19,Tg1016h21,Wah03,Rah03,Rc0416h02,Wah21,Rah06,Rah21,Rc0416h24,Tah24,Tg1016h20,Rah02,Rah20,Wah01,Rc0416h03,Rc0416h21,Se0716h19,Tah03,Tah04,Wah04,Rah01,Rah04,Rc0416h01,Rc0416h04,Se0716h02,Se0716h20,Tah06,Wah23,Wb0121h20,Sah04,Se0716h24,Tah02,Tah05,Tg1016h03,Tg1016h04,Wah05,Tah20,Tg1016h23,Wah24,Wb0121h02,Wb0121h06,Rc0416h05,Se0716h06,Tg1016h06,Wb0121h03,Wb0121h04</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>Sah04,Se0716h24,Tah02,Tah05,Tg1016h03,Tg1016h04,Wah05,Rah05,Rc0416h06,Rc0416h22,Rc0416h23,Sah20,Sah21,Sah22,Se0716h21,Tg1016h24,Wah20,Wb0121h21,Wb0121h23,Rah01,Rah04,Rc0416h01,Rc0416h04,Se0716h02,Se0716h20,Tah06,Wah23,Wb0121h20,Rc0416h05,Se0716h06,Tg1016h06,Wb0121h03,Wb0121h04,Rah23,Rah24,Sah03,Sah05,Sah19,Wah22,Rah03,Rc0416h02,Wah21,Sah23,Sah24,Se0716h04,Tg1016h01,Wah02,Wah19,Wb0121h01,Tah20,Tg1016h23,Wah24,Wb0121h02,Wb0121h06,Rah02,Rah20,Wah01,Se0716h23,Tg1016h19,Tg1016h21,Wah03,Rah06,Rah21,Rc0416h24,Tah24,Tg1016h20,Rc0416h20,Se0716h22,Tg1016h02,Tg1016h22,Wah06,Rc0416h03,Rc0416h21,Se0716h19,Tah03,Tah04,Wah04,Rah19,Se0716h01,Se0716h03,Se0716h05,Tah01,Tah19,Tah22,Rah22,Sah02,Sah06,Tah23,Wb0121h19,Wb0121h22,Rc0416h19,Sah01,Tah21,Tg1016h05,Wb0121h05,Wb0121h24</v>
+        <v>Rc0416h20,Se0716h22,Tg1016h02,Tg1016h22,Wah06,Rah22,Sah02,Sah06,Tah23,Wb0121h19,Wb0121h22,Rah05,Rc0416h06,Rc0416h22,Rc0416h23,Sah20,Sah21,Sah22,Se0716h21,Tg1016h24,Wah20,Wb0121h21,Wb0121h23,Sah23,Sah24,Se0716h04,Tg1016h01,Wah02,Wah19,Wb0121h01,Rah23,Rah24,Sah03,Sah05,Sah19,Wah22,Rc0416h19,Sah01,Tah21,Tg1016h05,Wb0121h05,Wb0121h24,Rah19,Se0716h01,Se0716h03,Se0716h05,Tah01,Tah19,Tah22,Se0716h23,Tg1016h19,Tg1016h21,Wah03,Rah03,Rc0416h02,Wah21,Rah06,Rah21,Rc0416h24,Tah24,Tg1016h20,Rah02,Rah20,Wah01,Rc0416h03,Rc0416h21,Se0716h19,Tah03,Tah04,Wah04,Rah01,Rah04,Rc0416h01,Rc0416h04,Se0716h02,Se0716h20,Tah06,Wah23,Wb0121h20,Sah04,Se0716h24,Tah02,Tah05,Tg1016h03,Tg1016h04,Wah05,Tah20,Tg1016h23,Wah24,Wb0121h02,Wb0121h06,Rc0416h05,Se0716h06,Tg1016h06,Wb0121h03,Wb0121h04</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Rah18,Rc0416h11,Wb0121h13,Rc0416h14,Rc0416h17,Sah10,Se0716h18,Tah09,Tg1016h11,Rc0416h07,Sah13,Sah16,Tg1016h13,Wah07,Wah16,Wb0121h09,Rah16,Sah08,Tah17,Wb0121h15,Wb0121h17,Rah07,Rc0416h08,Se0716h15,Se0716h17,Tg1016h14,Tg1016h15,Tg1016h16,Tg1016h17,Wah09,Wb0121h10,Rc0416h09,Sah07,Tah16,Tah18,Wah15,Wb0121h14,Wb0121h16,Rah17,Rc0416h10,Se0716h07,Tah11,Wb0121h12,Sah12,Se0716h09,Se0716h11,Tah10,Wb0121h11,Rah08,Rah10,Rc0416h16,Sah14,Sah17,Sah18,Se0716h12,Tah15,Tg1016h08,Wah08,Wah18,Sah15,Se0716h08,Se0716h13,Tg1016h09,Wah13,Rah15,Sah09,Rah13,Tah08,Wb0121h07,Rc0416h12,Se0716h10,Tg1016h07,Wah11,Rc0416h18,Se0716h14,Tah07,Tah12,Tg1016h12,Wah17,Rah12,Rah14,Rc0416h13,Tah13,Tg1016h18,Wah12,Rah09,Rah11,Rc0416h15,Sah11,Se0716h16,Tah14,Tg1016h10,Wah10,Wah14,Wb0121h08,Wb0121h18</v>
+        <v>Rah13,Tah08,Wb0121h07,Rah12,Rah14,Rc0416h13,Tah13,Tg1016h18,Wah12,Rc0416h14,Rc0416h17,Sah10,Se0716h18,Tah09,Tg1016h11,Rah17,Rc0416h10,Se0716h07,Tah11,Wb0121h12,Rah07,Rc0416h08,Se0716h15,Se0716h17,Tg1016h14,Tg1016h15,Tg1016h16,Tg1016h17,Wah09,Wb0121h10,Rah09,Rah11,Rc0416h15,Sah11,Se0716h16,Tah14,Tg1016h10,Wah10,Wah14,Wb0121h08,Wb0121h18,Rc0416h18,Se0716h14,Tah07,Tah12,Tg1016h12,Wah17,Sah15,Se0716h08,Se0716h13,Tg1016h09,Wah13,Rc0416h09,Sah07,Tah16,Tah18,Wah15,Wb0121h14,Wb0121h16,Rah15,Sah09,Rah08,Rah10,Rc0416h16,Sah14,Sah17,Sah18,Se0716h12,Tah15,Tg1016h08,Wah08,Wah18,Rc0416h12,Se0716h10,Tg1016h07,Wah11,Rc0416h07,Sah13,Sah16,Tg1016h13,Wah07,Wah16,Wb0121h09,Rah18,Rc0416h11,Wb0121h13,Sah12,Se0716h09,Se0716h11,Tah10,Wb0121h11,Rah16,Sah08,Tah17,Wb0121h15,Wb0121h17</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -3313,7 +3313,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D0BA86-6709-41CE-8AB6-950F12848CC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF93DF1F-60F0-4502-B6D5-7601A6E720A6}">
   <dimension ref="B2:F123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4695,7 +4695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E01F0D-F834-43AB-8E16-27FA6821E9F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62906A31-3EB3-4440-A95F-9E37E4183001}">
   <dimension ref="B2:O339"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11762,7 +11762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09AAB92-1992-4BAC-9524-4A0BCD7E06EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405B464C-09E4-4EB5-97AD-C7CF2F5E36DC}">
   <dimension ref="B2:O647"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>